<commit_message>
Fix empty Group Terminal Block names
Fix issue #616
</commit_message>
<xml_diff>
--- a/etc/Endpoint Name Testing.xlsx
+++ b/etc/Endpoint Name Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\microsoft\midi\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EB97E5-316D-4A3C-BA48-A80AB09D8158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B443B1F-7A7F-4B30-AF45-FD0C421FF866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27624" yWindow="672" windowWidth="32880" windowHeight="22104" xr2:uid="{37B460AA-2342-4D86-A85A-A889D9E438B4}"/>
+    <workbookView xWindow="27228" yWindow="12" windowWidth="34308" windowHeight="20352" xr2:uid="{37B460AA-2342-4D86-A85A-A889D9E438B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="150">
   <si>
     <t>Device</t>
   </si>
@@ -245,9 +245,6 @@
     <t>Serial number is in name, so if you have more than one of these, the second will have an incorrect name when using legacy-compatible WinMM names. Use new-style names to avoid this.</t>
   </si>
   <si>
-    <t>RME HDSPe MADI FX (PCIe)</t>
-  </si>
-  <si>
     <t>RME HDSPe MADI FX</t>
   </si>
   <si>
@@ -285,14 +282,276 @@
 Express  128: Port 8</t>
   </si>
   <si>
-    <t>Many other devices were tested but not recorded here</t>
+    <t>Generic silver with zipper cable</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0BFFQGB33</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B00007JRBM</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0DQYJJ3L2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0DM9LPSWQ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B09MTQ718H</t>
+  </si>
+  <si>
+    <t>KSA (MSFT driver)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B00967UN50</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B07T3R3WKD</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B071HPLJPZ</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B00D3QFHN8</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B00CO5IRSG</t>
+  </si>
+  <si>
+    <t>Donner Keyboard Controller</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0C1ZC45F5</t>
+  </si>
+  <si>
+    <t>DONNER N25</t>
+  </si>
+  <si>
+    <t>Many other devices, including Montage M, Roland A88, Waldorf Iridium, and others were tested but not recorded here</t>
+  </si>
+  <si>
+    <t>Conductive Labs MRCC</t>
+  </si>
+  <si>
+    <t>MRCC</t>
+  </si>
+  <si>
+    <t>MRCC
+MIDIIN2 (MRCC)
+MIDIIN3 (MRCC)
+…
+MIDIIN12 (MRCC)</t>
+  </si>
+  <si>
+    <t>Port 01
+Port 02
+Port 03
+… 
+Port 12</t>
+  </si>
+  <si>
+    <t>MRCC
+MIDIOUT2 (MRCC)
+MIDIOUT3 (MRCC)
+…
+MIDIOUT12 (MRCC)</t>
+  </si>
+  <si>
+    <t>This will have better names if you switch it to use new-style names</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>203 Matrix / Mystrix</t>
+  </si>
+  <si>
+    <t>https://203.io/</t>
+  </si>
+  <si>
+    <t>Bitwig Connect 4/12</t>
+  </si>
+  <si>
+    <t>Bitwig Connect</t>
+  </si>
+  <si>
+    <t>MIDI
+DAW</t>
+  </si>
+  <si>
+    <t>Another one that has better names if you use new-style names</t>
+  </si>
+  <si>
+    <t>Bitwig Connect
+MIDIIN2 (Bitwig Connect)</t>
+  </si>
+  <si>
+    <t>Bitwig Connect
+MIDIOUT2 (Bitwig Connect)</t>
+  </si>
+  <si>
+    <t>https://www.bitwig.com/connect/</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Zoom UAC-232</t>
+  </si>
+  <si>
+    <t>UAC2 / MIDI</t>
+  </si>
+  <si>
+    <t>ZOOM UAC-232</t>
+  </si>
+  <si>
+    <t>ZOOM UAC-232 MIDI I/O Port
+ZOOM UAC-232 for  Mix Control</t>
+  </si>
+  <si>
+    <t>Double space after "for" is part of the provided name.</t>
+  </si>
+  <si>
+    <t>MIDI Controller</t>
+  </si>
+  <si>
+    <t>MIDI Box</t>
+  </si>
+  <si>
+    <t>MIDI Cable</t>
+  </si>
+  <si>
+    <t>PCIe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RME HDSPe MADI FX </t>
+  </si>
+  <si>
+    <t>Synth</t>
+  </si>
+  <si>
+    <t>UAD Volt</t>
+  </si>
+  <si>
+    <t>Not enumerating. Needs investigation.</t>
+  </si>
+  <si>
+    <t>PreSonus Studio 24c</t>
+  </si>
+  <si>
+    <t>Studio 24c</t>
+  </si>
+  <si>
+    <t>Tascam US 2x2 HR</t>
+  </si>
+  <si>
+    <t>US-2x2HR MIDI</t>
+  </si>
+  <si>
+    <t>US-2x2HR MIDI MIDI IN</t>
+  </si>
+  <si>
+    <t>US-2x2HR MIDI MIDI OUT</t>
+  </si>
+  <si>
+    <t>Pin names include redundant "MIDI"</t>
+  </si>
+  <si>
+    <t>MOTU M4</t>
+  </si>
+  <si>
+    <t>Not class-compliant. Requires specific MOTU driver to be installed for MIDI to work.</t>
+  </si>
+  <si>
+    <t>Roli Lumi Keys (USB)</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>USB Audio Device</t>
+  </si>
+  <si>
+    <t>Generic name is unfortunate. It's set in the registry but not for the filter</t>
+  </si>
+  <si>
+    <t>ROLI LUMI Keys BLOCK</t>
+  </si>
+  <si>
+    <t>PreSonus Atom</t>
+  </si>
+  <si>
+    <t>ATOM</t>
+  </si>
+  <si>
+    <t>Donner Starrypad</t>
+  </si>
+  <si>
+    <t>STARRYPAD</t>
+  </si>
+  <si>
+    <t>M-Wave SMC Pad</t>
+  </si>
+  <si>
+    <t>SMC-PAD</t>
+  </si>
+  <si>
+    <t>SMC-PAD -Private
+SMC-PAD -Master
+SMC-PAD 3</t>
+  </si>
+  <si>
+    <t>SMC-PAD
+MIDIIN2 (SMC-PAD)
+MIDIIN3 (SMC-PAD)</t>
+  </si>
+  <si>
+    <t>SMC-PAD
+MIDIOUT2 (SMC-PAD)
+MIDIOUT3 (SMC-PAD)</t>
+  </si>
+  <si>
+    <t>Avatar EMP16 MIDI Pad</t>
+  </si>
+  <si>
+    <t>EMP-16</t>
+  </si>
+  <si>
+    <t>Arturia MiniFuse 4</t>
+  </si>
+  <si>
+    <t>Ships in an unusable state until you install Arturia software. Non-starter for Arm64.</t>
+  </si>
+  <si>
+    <t>Onyx Producer 2-2</t>
+  </si>
+  <si>
+    <t>Behringer UMC204HD</t>
+  </si>
+  <si>
+    <t>MIDI Endpoint has a Code 10 error and does not enumerate.  USB Audio 2 enumerates properly, though, just not MIDI 1.0. Fix: Manually assigning the MIDI 2.0 class driver with this enumerates properly.</t>
+  </si>
+  <si>
+    <t>UMC204HD 192k</t>
+  </si>
+  <si>
+    <t>Mackie ONYX Producer 2-2 + MIDI</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Mackie-Interface-Onyx-Producer-2-2/dp/B076646D8H</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Behringer-UMC204HD-BEHRINGER/dp/B00QHURLCW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +572,13 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -341,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,6 +633,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,84 +972,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E7D492-3ACB-4EC0-AB33-EA10494D9108}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="41.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="66.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="33.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="66.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="42.33203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="J1" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="3"/>
+      <c r="J2" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -791,18 +1074,22 @@
       <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -814,16 +1101,20 @@
       <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>110</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -837,16 +1128,23 @@
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>110</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>13</v>
@@ -860,16 +1158,20 @@
       <c r="G6" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>110</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>15</v>
@@ -883,16 +1185,23 @@
       <c r="G7" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>110</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>16</v>
@@ -906,16 +1215,23 @@
       <c r="G8" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>110</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>18</v>
@@ -929,19 +1245,25 @@
       <c r="G9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J9" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>110</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>13</v>
@@ -955,16 +1277,23 @@
       <c r="G10" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>110</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>23</v>
@@ -978,65 +1307,76 @@
       <c r="G11" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="H11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>30</v>
       </c>
       <c r="G13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>40</v>
+        <v>110</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>40</v>
@@ -1050,91 +1390,117 @@
       <c r="G14" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="H14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="I15" s="3"/>
+      <c r="J15" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="66" x14ac:dyDescent="0.3">
+      <c r="J16" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>53</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J17" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>58</v>
+        <v>108</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>58</v>
@@ -1148,268 +1514,817 @@
       <c r="G18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="F19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="5" t="s">
+    </row>
+    <row r="20" spans="1:10" ht="66" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="5" t="s">
+    </row>
+    <row r="21" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="J22" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="66" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="4"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="5"/>
+      <c r="I27" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C39" s="2"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C40" s="2"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C41" s="2"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="4"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C43" s="6"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D63" s="6"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Various changes to update to VS26
</commit_message>
<xml_diff>
--- a/etc/Endpoint Name Testing.xlsx
+++ b/etc/Endpoint Name Testing.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\microsoft\midi\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B9CD4-B495-4A57-B5A0-7874B917828C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3786DEE8-587C-4204-8C68-8B85E1EABA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26784" yWindow="624" windowWidth="33096" windowHeight="24540" xr2:uid="{37B460AA-2342-4D86-A85A-A889D9E438B4}"/>
+    <workbookView xWindow="29964" yWindow="84" windowWidth="31524" windowHeight="25080" xr2:uid="{37B460AA-2342-4D86-A85A-A889D9E438B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="156">
   <si>
     <t>Device</t>
   </si>
@@ -546,6 +545,24 @@
   </si>
   <si>
     <t>Smart Cable</t>
+  </si>
+  <si>
+    <t>Waldorf Iridium Desktop</t>
+  </si>
+  <si>
+    <t>Synthesizer</t>
+  </si>
+  <si>
+    <t>Iridium</t>
+  </si>
+  <si>
+    <t>(bidirectional FB) Synth</t>
+  </si>
+  <si>
+    <t>Iridium (MIDI 2.0)</t>
+  </si>
+  <si>
+    <t>Using MIDI 2.0 firmware.</t>
   </si>
 </sst>
 </file>
@@ -974,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E7D492-3ACB-4EC0-AB33-EA10494D9108}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B37"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2079,15 +2096,33 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="3"/>
+      <c r="A39" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>

</xml_diff>